<commit_message>
Added url to wireframe workbook
</commit_message>
<xml_diff>
--- a/Design/UI/Wireframes/Wireframe Elements.xlsx
+++ b/Design/UI/Wireframes/Wireframe Elements.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
-  <si>
-    <t>Wireframes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Component Name</t>
   </si>
@@ -102,16 +99,30 @@
   </si>
   <si>
     <t>Bread Crumb Area</t>
+  </si>
+  <si>
+    <t>Wireframe</t>
+  </si>
+  <si>
+    <t>https://wireframe.cc/Hpuwsw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,13 +145,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,7 +436,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,113 +451,119 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>